<commit_message>
AIP-391 AIP-462 Updated code as per the review and created one test case BTC-639 as well according to review comments, now as per code we can verify trigger priority on configuration page for boundary value and also verify trigger priority by sending FR manual trigger and checking the priority on DFR pop-up and on PDP page.
</commit_message>
<xml_diff>
--- a/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_114.xlsx
+++ b/Carrick_AutomatedTest/Carrick_Automation/TestData/BTC_114.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B106DA6B-012C-4078-B256-0E998DF8F594}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED1E3F3-EDF1-446F-9DC6-5B04947FA522}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
     <t>DeviceName</t>
   </si>
@@ -52,28 +52,22 @@
     <t>10.75.58.51</t>
   </si>
   <si>
-    <t>PrefaultTime</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>TriggerPriority_Min</t>
-  </si>
-  <si>
-    <t>TriggerPriority_Max</t>
-  </si>
-  <si>
-    <t>TriggerPriority_Mid</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>51</t>
-  </si>
-  <si>
-    <t>101</t>
+    <t>TriggerPriority</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>64</t>
   </si>
 </sst>
 </file>
@@ -395,7 +389,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,17 +425,10 @@
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" t="s">
         <v>10</v>
       </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -463,46 +450,116 @@
         <v>409026540</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1">
+        <v>409026540</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>

</xml_diff>